<commit_message>
Finished 2011-12, 2012-13 lists of lesions n=526
</commit_message>
<xml_diff>
--- a/For Cristina_MRI's_Path_Nov 2014.xlsx
+++ b/For Cristina_MRI's_Path_Nov 2014.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="18975" windowHeight="11955" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="18975" windowHeight="8295" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="noMRN" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="troubleshooting" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -134,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="168">
   <si>
     <t>MRN #</t>
   </si>
@@ -410,9 +410,6 @@
   </si>
   <si>
     <t xml:space="preserve">IDC </t>
-  </si>
-  <si>
-    <t>2013-May-25</t>
   </si>
   <si>
     <t>2012-May-08</t>
@@ -574,13 +571,97 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>NOTES</t>
+  </si>
+  <si>
+    <t>Not in biomatrix, found different accesion for 15/11/2014</t>
+  </si>
+  <si>
+    <t>used assession  5186978</t>
+  </si>
+  <si>
+    <t>need assesion 7080675, but NOT FOUND IN ASOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">not in biomatrix </t>
+  </si>
+  <si>
+    <t>Changed asccession to 6983262</t>
+  </si>
+  <si>
+    <t>aca1</t>
+  </si>
+  <si>
+    <t># Missing areas (could be entered as "non-mass") In the right breast, image 72, 2 areas of enhancement, the first one measuring 6 mm centrally and the second one at 6 o'clock measuring 3 mm.  They both show washout on delayed phase.  No corresponding T2.  They are 17 mm apart.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DUCTAL HYPERPLASIA </t>
+  </si>
+  <si>
+    <t># no findings in MRI?</t>
+  </si>
+  <si>
+    <t># calcifications biopsied on left breast not seen in MRI</t>
+  </si>
+  <si>
+    <t>benign  - no findings in rad report ?</t>
+  </si>
+  <si>
+    <t># No procedure done within 3 months from imaging</t>
+  </si>
+  <si>
+    <t>ADH and DCIS  # missing finding in biomatrix. In the right upper inner quadrant image 73 there is a new heterogeneously enhancing 5 mm mass with rapid early and delayed washout with an isointense T2 signal.</t>
+  </si>
+  <si>
+    <t>Part B - Left breast biopsy, left upper inner breast:   - DENSE FIBROSIS AND FOCAL SCLEROSING ADENOSIS WITH FOCAL     CALCIFICATION"</t>
+  </si>
+  <si>
+    <t>CADid</t>
+  </si>
+  <si>
+    <t>DateofExam</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Accession#</t>
+  </si>
+  <si>
+    <t># not found in AS0SUN</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> C.  Left breast lump:  INFILTRATING DUCT CARCINOMA NOS</t>
+  </si>
+  <si>
+    <t># no assession in AS0SUNB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATYPICAL LOBULAR HYPERPLASIA                    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROLIFERATIVE FIBROCYSTIC CHANGES     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  # NOT FOUND IN AS0SUNB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">left fibrocystic changes                </t>
+  </si>
+  <si>
+    <t># NOT FOUND IN AS0SUNB</t>
+  </si>
+  <si>
+    <t># not entered in BIOMATRIX yet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -614,8 +695,21 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -640,8 +734,25 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -649,11 +760,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -709,8 +836,37 @@
     <xf numFmtId="14" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1006,8 +1162,8 @@
   <dimension ref="A1:H120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A99" sqref="A99:F120"/>
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1022,9 +1178,9 @@
     <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>0</v>
@@ -1041,8 +1197,11 @@
       <c r="F1" s="8" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" s="3" customFormat="1">
+      <c r="G1" s="21" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="3" customFormat="1">
       <c r="A2" s="10"/>
       <c r="B2" s="10" t="s">
         <v>66</v>
@@ -1054,7 +1213,7 @@
       <c r="E2" s="11"/>
       <c r="F2" s="10"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" s="7">
         <v>411</v>
       </c>
@@ -1074,7 +1233,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4" s="7">
         <v>412</v>
       </c>
@@ -1094,7 +1253,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:7">
       <c r="A5" s="7">
         <v>413</v>
       </c>
@@ -1114,7 +1273,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:7">
       <c r="A6" s="7">
         <v>414</v>
       </c>
@@ -1134,7 +1293,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:7">
       <c r="A7" s="7">
         <v>415</v>
       </c>
@@ -1154,7 +1313,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:7">
       <c r="A8" s="7">
         <v>416</v>
       </c>
@@ -1171,10 +1330,10 @@
         <v>40798</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="7">
         <v>417</v>
       </c>
@@ -1194,7 +1353,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:7">
       <c r="A10" s="7">
         <v>418</v>
       </c>
@@ -1214,7 +1373,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:7">
       <c r="A11" s="7">
         <v>419</v>
       </c>
@@ -1231,10 +1390,10 @@
         <v>41328</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="7">
         <v>420</v>
       </c>
@@ -1254,7 +1413,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:7">
       <c r="A13" s="7">
         <v>421</v>
       </c>
@@ -1274,7 +1433,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:7">
       <c r="A14" s="7">
         <v>422</v>
       </c>
@@ -1294,7 +1453,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:7">
       <c r="A15" s="7">
         <v>423</v>
       </c>
@@ -1314,7 +1473,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:7">
       <c r="A16" s="7">
         <v>424</v>
       </c>
@@ -1334,7 +1493,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:7">
       <c r="A17" s="7">
         <v>425</v>
       </c>
@@ -1354,7 +1513,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:7">
       <c r="A18" s="7">
         <v>426</v>
       </c>
@@ -1374,7 +1533,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:7">
       <c r="A19" s="7">
         <v>427</v>
       </c>
@@ -1394,7 +1553,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:7">
       <c r="A20" s="7">
         <v>428</v>
       </c>
@@ -1414,7 +1573,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:7">
       <c r="A21" s="7">
         <v>429</v>
       </c>
@@ -1431,10 +1590,10 @@
         <v>40819</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="7">
         <v>430</v>
       </c>
@@ -1454,7 +1613,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:7">
       <c r="A23" s="7">
         <v>431</v>
       </c>
@@ -1474,7 +1633,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:7">
       <c r="A24" s="7">
         <v>432</v>
       </c>
@@ -1494,7 +1653,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:7">
       <c r="A25" s="7">
         <v>433</v>
       </c>
@@ -1514,7 +1673,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:7">
       <c r="A26" s="7">
         <v>434</v>
       </c>
@@ -1534,7 +1693,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:7">
       <c r="A27" s="7">
         <v>435</v>
       </c>
@@ -1554,7 +1713,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:7">
       <c r="A28" s="7">
         <v>436</v>
       </c>
@@ -1574,27 +1733,30 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="7">
+    <row r="29" spans="1:7">
+      <c r="A29" s="19">
         <v>437</v>
       </c>
-      <c r="B29" s="7">
+      <c r="B29" s="19">
         <v>2435265</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="19">
         <v>616</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="19">
         <v>8026103</v>
       </c>
-      <c r="E29" s="14">
+      <c r="E29" s="20">
         <v>41964</v>
       </c>
-      <c r="F29" s="7" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="F29" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" s="7">
         <v>438</v>
       </c>
@@ -1605,16 +1767,16 @@
         <v>3092</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E30" s="14">
         <v>39345</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" s="7">
         <v>439</v>
       </c>
@@ -1631,27 +1793,27 @@
         <v>39353</v>
       </c>
       <c r="F31" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="19">
+        <v>440</v>
+      </c>
+      <c r="B32" s="19">
+        <v>2470729</v>
+      </c>
+      <c r="C32" s="19">
+        <v>3093</v>
+      </c>
+      <c r="D32" s="19">
+        <v>7790909</v>
+      </c>
+      <c r="E32" s="20">
+        <v>41722</v>
+      </c>
+      <c r="F32" s="19" t="s">
         <v>109</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
-      <c r="A32" s="7">
-        <v>440</v>
-      </c>
-      <c r="B32" s="7">
-        <v>2470729</v>
-      </c>
-      <c r="C32" s="7">
-        <v>3093</v>
-      </c>
-      <c r="D32" s="7">
-        <v>7790909</v>
-      </c>
-      <c r="E32" s="14">
-        <v>41722</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1671,47 +1833,50 @@
         <v>40924</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:8">
-      <c r="A34" s="7">
+      <c r="A34" s="19">
         <v>442</v>
       </c>
-      <c r="B34" s="12">
+      <c r="B34" s="19">
         <v>2565945</v>
       </c>
-      <c r="C34" s="12">
+      <c r="C34" s="19">
         <v>2042</v>
       </c>
-      <c r="D34" s="7">
+      <c r="D34" s="19">
         <v>4907456</v>
       </c>
-      <c r="E34" s="14">
+      <c r="E34" s="20">
         <v>39882</v>
       </c>
-      <c r="F34" s="7" t="s">
-        <v>102</v>
+      <c r="F34" s="19" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="35" spans="1:8">
-      <c r="A35" s="7">
+      <c r="A35" s="19">
         <v>443</v>
       </c>
-      <c r="B35" s="12">
+      <c r="B35" s="19">
         <v>2565945</v>
       </c>
-      <c r="C35" s="12">
+      <c r="C35" s="19">
         <v>2042</v>
       </c>
-      <c r="D35" s="7">
+      <c r="D35" s="19">
         <v>7062134</v>
       </c>
-      <c r="E35" s="14">
+      <c r="E35" s="20">
         <v>40970</v>
       </c>
-      <c r="F35" s="7" t="s">
+      <c r="F35" s="19" t="s">
         <v>5</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -1731,11 +1896,11 @@
         <v>41736</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="37" spans="1:8">
-      <c r="A37" s="7">
+      <c r="A37" s="12">
         <v>445</v>
       </c>
       <c r="B37" s="12">
@@ -1744,37 +1909,37 @@
       <c r="C37" s="12">
         <v>3082</v>
       </c>
-      <c r="D37" s="7">
+      <c r="D37" s="12">
         <v>5378256</v>
       </c>
-      <c r="E37" s="14">
+      <c r="E37" s="13">
         <v>40445</v>
       </c>
-      <c r="F37" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="G37" s="7" t="s">
+      <c r="F37" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38" s="19">
+        <v>446</v>
+      </c>
+      <c r="B38" s="19">
+        <v>2581758</v>
+      </c>
+      <c r="C38" s="19">
+        <v>3082</v>
+      </c>
+      <c r="D38" s="19">
+        <v>7101412</v>
+      </c>
+      <c r="E38" s="20">
+        <v>41001</v>
+      </c>
+      <c r="F38" s="19" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="A38" s="7">
-        <v>446</v>
-      </c>
-      <c r="B38" s="12">
-        <v>2581758</v>
-      </c>
-      <c r="C38" s="12">
-        <v>3082</v>
-      </c>
-      <c r="D38" s="7">
-        <v>7101412</v>
-      </c>
-      <c r="E38" s="14">
-        <v>41001</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>113</v>
+      <c r="G38" s="22" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -1794,7 +1959,7 @@
         <v>40497</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:8">
@@ -1814,10 +1979,10 @@
         <v>41001</v>
       </c>
       <c r="F40" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="G40" s="7" t="s">
         <v>115</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -1837,7 +2002,7 @@
         <v>41964</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -1857,10 +2022,10 @@
         <v>40932</v>
       </c>
       <c r="F42" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="H42" s="7" t="s">
         <v>118</v>
-      </c>
-      <c r="H42" s="7" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -1878,7 +2043,7 @@
         <v>40947</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -1898,7 +2063,7 @@
         <v>40967</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -1918,7 +2083,7 @@
         <v>41667</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -1938,7 +2103,7 @@
         <v>40778</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -1952,33 +2117,36 @@
         <v>4039</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E47" s="14">
         <v>40952</v>
       </c>
       <c r="F47" s="7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="19">
+        <v>456</v>
+      </c>
+      <c r="B48" s="19">
+        <v>2798728</v>
+      </c>
+      <c r="C48" s="19">
+        <v>4016</v>
+      </c>
+      <c r="D48" s="19">
+        <v>7455946</v>
+      </c>
+      <c r="E48" s="20">
+        <v>41369</v>
+      </c>
+      <c r="F48" s="19" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="7">
-        <v>456</v>
-      </c>
-      <c r="B48" s="7">
-        <v>2798728</v>
-      </c>
-      <c r="C48" s="7">
-        <v>4016</v>
-      </c>
-      <c r="D48" s="7">
-        <v>7455946</v>
-      </c>
-      <c r="E48" s="14">
-        <v>41369</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>125</v>
+      <c r="G48" s="1" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -1998,30 +2166,30 @@
         <v>41008</v>
       </c>
       <c r="F49" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="19">
+        <v>458</v>
+      </c>
+      <c r="B50" s="19">
+        <v>2801064</v>
+      </c>
+      <c r="C50" s="19">
+        <v>4018</v>
+      </c>
+      <c r="D50" s="19">
+        <v>6983262</v>
+      </c>
+      <c r="E50" s="20">
+        <v>41621</v>
+      </c>
+      <c r="F50" s="19" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="50" spans="1:7">
-      <c r="A50" s="7">
-        <v>458</v>
-      </c>
-      <c r="B50" s="7">
-        <v>2801064</v>
-      </c>
-      <c r="C50" s="7">
-        <v>4018</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="E50" s="14">
-        <v>41621</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>127</v>
-      </c>
       <c r="G50" s="7" t="s">
-        <v>128</v>
+        <v>145</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -2061,7 +2229,7 @@
         <v>40928</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -2101,7 +2269,7 @@
         <v>41170</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="55" spans="1:7" s="2" customFormat="1">
@@ -2115,13 +2283,13 @@
         <v>4040</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E55" s="13">
         <v>40911</v>
       </c>
       <c r="F55" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -2141,7 +2309,7 @@
         <v>41093</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -2161,7 +2329,7 @@
         <v>40917</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -2181,7 +2349,7 @@
         <v>40981</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -2195,13 +2363,13 @@
         <v>4045</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E59" s="14">
         <v>41022</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -2215,13 +2383,13 @@
         <v>3078</v>
       </c>
       <c r="D60" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E60" s="14">
         <v>39874</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -2235,7 +2403,7 @@
         <v>3076</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E61" s="14">
         <v>40975</v>
@@ -2261,7 +2429,7 @@
         <v>41029</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -2279,7 +2447,7 @@
         <v>40942</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -2297,7 +2465,7 @@
         <v>40996</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -2337,10 +2505,10 @@
         <v>41733</v>
       </c>
       <c r="F66" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="G66" s="7" t="s">
         <v>135</v>
-      </c>
-      <c r="G66" s="7" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -2354,7 +2522,7 @@
         <v>3053</v>
       </c>
       <c r="D67" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E67" s="14">
         <v>41387</v>
@@ -2374,13 +2542,13 @@
         <v>3053</v>
       </c>
       <c r="D68" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E68" s="14">
         <v>40956</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -2414,13 +2582,13 @@
         <v>3046</v>
       </c>
       <c r="D70" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E70" s="14">
         <v>41296</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -2434,13 +2602,13 @@
         <v>3046</v>
       </c>
       <c r="D71" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E71" s="14">
         <v>41618</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -2942,7 +3110,7 @@
     <row r="99" spans="1:6" s="4" customFormat="1">
       <c r="A99" s="17"/>
       <c r="B99" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C99" s="17"/>
       <c r="D99" s="17"/>
@@ -3223,7 +3391,7 @@
         <v>7446343</v>
       </c>
       <c r="E113" s="14" t="s">
-        <v>92</v>
+        <v>146</v>
       </c>
       <c r="F113" s="7" t="s">
         <v>79</v>
@@ -3243,10 +3411,10 @@
         <v>7128025</v>
       </c>
       <c r="E114" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="F114" s="7" t="s">
         <v>93</v>
-      </c>
-      <c r="F114" s="7" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="115" spans="1:6">
@@ -3263,7 +3431,7 @@
         <v>7581124</v>
       </c>
       <c r="E115" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F115" s="7" t="s">
         <v>79</v>
@@ -3283,10 +3451,10 @@
         <v>5435020</v>
       </c>
       <c r="E116" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="F116" s="7" t="s">
         <v>96</v>
-      </c>
-      <c r="F116" s="7" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="117" spans="1:6">
@@ -3303,10 +3471,10 @@
         <v>6971531</v>
       </c>
       <c r="E117" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="F117" s="7" t="s">
         <v>98</v>
-      </c>
-      <c r="F117" s="7" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="118" spans="1:6">
@@ -3323,10 +3491,10 @@
         <v>7742881</v>
       </c>
       <c r="E118" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="F118" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="F118" s="7" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="119" spans="1:6">
@@ -3346,7 +3514,7 @@
         <v>87</v>
       </c>
       <c r="F119" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="120" spans="1:6">
@@ -3363,7 +3531,7 @@
         <v>5021830</v>
       </c>
       <c r="E120" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F120" s="7" t="s">
         <v>79</v>
@@ -3380,7 +3548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A99" sqref="A99:H120"/>
     </sheetView>
   </sheetViews>
@@ -3392,7 +3560,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -3531,7 +3699,7 @@
         <v>40798</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -3588,7 +3756,7 @@
         <v>41328</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -3778,7 +3946,7 @@
         <v>40819</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -3930,7 +4098,7 @@
         <v>41964</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
@@ -3943,13 +4111,13 @@
         <v>3092</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D30" s="14">
         <v>39345</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -3968,7 +4136,7 @@
         <v>39353</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
@@ -3987,7 +4155,7 @@
         <v>41722</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
@@ -4006,7 +4174,7 @@
         <v>40924</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
@@ -4025,7 +4193,7 @@
         <v>39882</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
@@ -4063,7 +4231,7 @@
         <v>41736</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
@@ -4082,10 +4250,10 @@
         <v>40445</v>
       </c>
       <c r="E37" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="F37" s="7" t="s">
         <v>111</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>112</v>
       </c>
       <c r="G37" s="1"/>
     </row>
@@ -4103,7 +4271,7 @@
         <v>41001</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
@@ -4122,7 +4290,7 @@
         <v>40497</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
@@ -4141,10 +4309,10 @@
         <v>41001</v>
       </c>
       <c r="E40" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F40" s="7" t="s">
         <v>115</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>116</v>
       </c>
       <c r="G40" s="1"/>
     </row>
@@ -4162,7 +4330,7 @@
         <v>41964</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
@@ -4181,11 +4349,11 @@
         <v>40932</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F42" s="1"/>
       <c r="G42" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -4200,7 +4368,7 @@
         <v>40947</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
@@ -4219,7 +4387,7 @@
         <v>40967</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
@@ -4238,7 +4406,7 @@
         <v>41667</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
@@ -4257,7 +4425,7 @@
         <v>40778</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
@@ -4270,13 +4438,13 @@
         <v>4039</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D47" s="14">
         <v>40952</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
@@ -4295,7 +4463,7 @@
         <v>41369</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
@@ -4314,7 +4482,7 @@
         <v>41008</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
@@ -4327,16 +4495,16 @@
         <v>4018</v>
       </c>
       <c r="C50" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D50" s="14">
         <v>41621</v>
       </c>
       <c r="E50" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="F50" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="F50" s="7" t="s">
-        <v>128</v>
       </c>
       <c r="G50" s="1"/>
     </row>
@@ -4373,7 +4541,7 @@
         <v>40928</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
@@ -4411,7 +4579,7 @@
         <v>41170</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
@@ -4424,13 +4592,13 @@
         <v>4040</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D55" s="13">
         <v>40911</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
@@ -4449,7 +4617,7 @@
         <v>41093</v>
       </c>
       <c r="E56" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
@@ -4468,7 +4636,7 @@
         <v>40917</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
@@ -4487,7 +4655,7 @@
         <v>40981</v>
       </c>
       <c r="E58" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
@@ -4500,13 +4668,13 @@
         <v>4045</v>
       </c>
       <c r="C59" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D59" s="14">
         <v>41022</v>
       </c>
       <c r="E59" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
@@ -4519,13 +4687,13 @@
         <v>3078</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D60" s="14">
         <v>39874</v>
       </c>
       <c r="E60" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
@@ -4538,7 +4706,7 @@
         <v>3076</v>
       </c>
       <c r="C61" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D61" s="14">
         <v>40975</v>
@@ -4563,7 +4731,7 @@
         <v>41029</v>
       </c>
       <c r="E62" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
@@ -4580,7 +4748,7 @@
         <v>40942</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
@@ -4597,7 +4765,7 @@
         <v>40996</v>
       </c>
       <c r="E64" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
@@ -4635,10 +4803,10 @@
         <v>41733</v>
       </c>
       <c r="E66" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="F66" s="7" t="s">
         <v>135</v>
-      </c>
-      <c r="F66" s="7" t="s">
-        <v>136</v>
       </c>
       <c r="G66" s="1"/>
     </row>
@@ -4650,7 +4818,7 @@
         <v>3053</v>
       </c>
       <c r="C67" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D67" s="14">
         <v>41387</v>
@@ -4669,13 +4837,13 @@
         <v>3053</v>
       </c>
       <c r="C68" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D68" s="14">
         <v>40956</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
@@ -4707,13 +4875,13 @@
         <v>3046</v>
       </c>
       <c r="C70" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D70" s="14">
         <v>41296</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
@@ -4726,13 +4894,13 @@
         <v>3046</v>
       </c>
       <c r="C71" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D71" s="14">
         <v>41618</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
@@ -5160,7 +5328,7 @@
     <row r="99" spans="1:6">
       <c r="A99" s="17"/>
       <c r="B99" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C99" s="17"/>
       <c r="D99" s="17"/>
@@ -5419,7 +5587,7 @@
         <v>41037</v>
       </c>
       <c r="E114" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -5453,7 +5621,7 @@
         <v>40493</v>
       </c>
       <c r="E116" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="117" spans="1:5">
@@ -5470,7 +5638,7 @@
         <v>41023</v>
       </c>
       <c r="E117" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="118" spans="1:5">
@@ -5487,7 +5655,7 @@
         <v>41782</v>
       </c>
       <c r="E118" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="119" spans="1:5">
@@ -5504,7 +5672,7 @@
         <v>41034</v>
       </c>
       <c r="E119" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="120" spans="1:5">
@@ -5532,12 +5700,306 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A2:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="23"/>
+    <col min="2" max="2" width="13.28515625" style="23" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" style="23" customWidth="1"/>
+    <col min="4" max="4" width="61" style="23" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7">
+      <c r="A2" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="B2" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="D2" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="23">
+        <v>3026</v>
+      </c>
+      <c r="B3" s="23">
+        <v>6830523</v>
+      </c>
+      <c r="C3" s="25">
+        <v>40717</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="23">
+        <v>710</v>
+      </c>
+      <c r="B4" s="23">
+        <v>6798490</v>
+      </c>
+      <c r="C4" s="25">
+        <v>40694</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="23">
+        <v>4018</v>
+      </c>
+      <c r="B5" s="23">
+        <v>6983262</v>
+      </c>
+      <c r="C5" s="25">
+        <v>40872</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="23">
+        <v>3062</v>
+      </c>
+      <c r="B6" s="23">
+        <v>7054872</v>
+      </c>
+      <c r="C6" s="25">
+        <v>40968</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="23">
+        <v>3027</v>
+      </c>
+      <c r="B7" s="23">
+        <v>7652412</v>
+      </c>
+      <c r="C7" s="25">
+        <v>41721</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="23">
+        <v>944</v>
+      </c>
+      <c r="B8" s="23">
+        <v>7742881</v>
+      </c>
+      <c r="C8" s="25">
+        <v>41782</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="B11" s="28"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="23">
+        <v>3039</v>
+      </c>
+      <c r="B13" s="23">
+        <v>3628156</v>
+      </c>
+      <c r="C13" s="25">
+        <v>38405</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="23">
+        <v>3082</v>
+      </c>
+      <c r="B14" s="23">
+        <v>7080675</v>
+      </c>
+      <c r="C14" s="25">
+        <v>40988</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="23">
+        <v>6148</v>
+      </c>
+      <c r="B15" s="23">
+        <v>3512706</v>
+      </c>
+      <c r="C15" s="25">
+        <v>38265</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>160</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="23">
+        <v>2042</v>
+      </c>
+      <c r="B16" s="23">
+        <v>4861891</v>
+      </c>
+      <c r="C16" s="25">
+        <v>39836</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>156</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="23">
+        <v>616</v>
+      </c>
+      <c r="B21" s="23">
+        <v>8026103</v>
+      </c>
+      <c r="C21" s="25">
+        <v>41964</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="23">
+        <v>3092</v>
+      </c>
+      <c r="B22" s="23">
+        <v>4473234</v>
+      </c>
+      <c r="C22" s="25">
+        <v>39353</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="23">
+        <v>3097</v>
+      </c>
+      <c r="B23" s="23">
+        <v>7024601</v>
+      </c>
+      <c r="C23" s="25">
+        <v>40924</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="23">
+        <v>4016</v>
+      </c>
+      <c r="B24" s="23">
+        <v>7455946</v>
+      </c>
+      <c r="C24" s="25">
+        <v>41369</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>124</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>